<commit_message>
Commit with causal arima plot working
</commit_message>
<xml_diff>
--- a/Outputs/WY/Results.xlsx
+++ b/Outputs/WY/Results.xlsx
@@ -437,16 +437,16 @@
         <v>11</v>
       </c>
       <c r="D2" t="n">
-        <v>-0.634571743841126</v>
+        <v>4.55194436134888</v>
       </c>
       <c r="E2" t="n">
-        <v>-6.89955769228011</v>
+        <v>0.0563609197510995</v>
       </c>
       <c r="F2" t="n">
-        <v>6.31429715638182</v>
+        <v>9.45954957352126</v>
       </c>
       <c r="G2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H2" t="n">
         <v>1572.84210526316</v>
@@ -466,13 +466,13 @@
         <v>12</v>
       </c>
       <c r="D3" t="n">
-        <v>-11.6326171443048</v>
+        <v>-1.648950251367</v>
       </c>
       <c r="E3" t="n">
-        <v>-26.3956588080779</v>
+        <v>-13.5052864425289</v>
       </c>
       <c r="F3" t="n">
-        <v>10.8466516132712</v>
+        <v>11.2187000547253</v>
       </c>
       <c r="G3" t="n">
         <v>0</v>
@@ -495,13 +495,13 @@
         <v>13</v>
       </c>
       <c r="D4" t="n">
-        <v>-11.878228791999</v>
+        <v>-6.97982475932386</v>
       </c>
       <c r="E4" t="n">
-        <v>-25.1742724200863</v>
+        <v>-16.6459358443617</v>
       </c>
       <c r="F4" t="n">
-        <v>6.55360274092828</v>
+        <v>4.74889646073614</v>
       </c>
       <c r="G4" t="n">
         <v>0</v>
@@ -524,13 +524,13 @@
         <v>14</v>
       </c>
       <c r="D5" t="n">
-        <v>-13.6992056131681</v>
+        <v>-1.44699984262765</v>
       </c>
       <c r="E5" t="n">
-        <v>-36.3308687298679</v>
+        <v>-19.6318810745464</v>
       </c>
       <c r="F5" t="n">
-        <v>25.0810271482947</v>
+        <v>21.0400122736455</v>
       </c>
       <c r="G5" t="n">
         <v>0</v>
@@ -553,13 +553,13 @@
         <v>15</v>
       </c>
       <c r="D6" t="n">
-        <v>-45.3674498379461</v>
+        <v>-45.9166131821395</v>
       </c>
       <c r="E6" t="n">
-        <v>-55.4288568794327</v>
+        <v>-52.1196125977235</v>
       </c>
       <c r="F6" t="n">
-        <v>-31.1172705492752</v>
+        <v>-38.2501219701516</v>
       </c>
       <c r="G6" t="n">
         <v>1</v>
@@ -582,13 +582,13 @@
         <v>11</v>
       </c>
       <c r="D7" t="n">
-        <v>12.9460632445514</v>
+        <v>20.3167387785498</v>
       </c>
       <c r="E7" t="n">
-        <v>1.83706219631042</v>
+        <v>13.2842041030328</v>
       </c>
       <c r="F7" t="n">
-        <v>27.961155665519</v>
+        <v>28.686158084496</v>
       </c>
       <c r="G7" t="n">
         <v>1</v>
@@ -611,16 +611,16 @@
         <v>12</v>
       </c>
       <c r="D8" t="n">
-        <v>9.83012425585809</v>
+        <v>21.3210454396107</v>
       </c>
       <c r="E8" t="n">
-        <v>-4.65886107605062</v>
+        <v>12.0020624217291</v>
       </c>
       <c r="F8" t="n">
-        <v>28.8412377121439</v>
+        <v>31.4976304702006</v>
       </c>
       <c r="G8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H8" t="n">
         <v>1118.15789473684</v>
@@ -640,13 +640,13 @@
         <v>13</v>
       </c>
       <c r="D9" t="n">
-        <v>35.6085858857582</v>
+        <v>57.6830514671484</v>
       </c>
       <c r="E9" t="n">
-        <v>2.83000659333597</v>
+        <v>31.8625096642734</v>
       </c>
       <c r="F9" t="n">
-        <v>88.265312934087</v>
+        <v>91.9316233452192</v>
       </c>
       <c r="G9" t="n">
         <v>1</v>
@@ -669,16 +669,16 @@
         <v>14</v>
       </c>
       <c r="D10" t="n">
-        <v>29.0819195352058</v>
+        <v>56.8380396682825</v>
       </c>
       <c r="E10" t="n">
-        <v>-1.84390981975938</v>
+        <v>29.6456058789541</v>
       </c>
       <c r="F10" t="n">
-        <v>75.2410027747163</v>
+        <v>90.2060849455851</v>
       </c>
       <c r="G10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H10" t="n">
         <v>266.157894736842</v>
@@ -698,13 +698,13 @@
         <v>15</v>
       </c>
       <c r="D11" t="n">
-        <v>-22.752259021006</v>
+        <v>-16.5365931509972</v>
       </c>
       <c r="E11" t="n">
-        <v>-34.364357409868</v>
+        <v>-25.1675826809712</v>
       </c>
       <c r="F11" t="n">
-        <v>-7.96374885327508</v>
+        <v>-5.90321396800044</v>
       </c>
       <c r="G11" t="n">
         <v>1</v>
@@ -727,13 +727,13 @@
         <v>11</v>
       </c>
       <c r="D12" t="n">
-        <v>1.72879236219983</v>
+        <v>3.39013510432004</v>
       </c>
       <c r="E12" t="n">
-        <v>-4.04380842808095</v>
+        <v>-0.692014453713557</v>
       </c>
       <c r="F12" t="n">
-        <v>8.01691474887901</v>
+        <v>7.89734044144451</v>
       </c>
       <c r="G12" t="n">
         <v>0</v>
@@ -756,16 +756,16 @@
         <v>12</v>
       </c>
       <c r="D13" t="n">
-        <v>7.18738500644974</v>
+        <v>19.8336351311463</v>
       </c>
       <c r="E13" t="n">
-        <v>-10.2563553073949</v>
+        <v>7.29071820799665</v>
       </c>
       <c r="F13" t="n">
-        <v>26.6892608985865</v>
+        <v>33.9609753181257</v>
       </c>
       <c r="G13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H13" t="n">
         <v>2220.52631578947</v>
@@ -785,13 +785,13 @@
         <v>13</v>
       </c>
       <c r="D14" t="n">
-        <v>64.359884180366</v>
+        <v>122.247679917388</v>
       </c>
       <c r="E14" t="n">
-        <v>8.01521178802268</v>
+        <v>65.5287541530487</v>
       </c>
       <c r="F14" t="n">
-        <v>171.718813969175</v>
+        <v>223.377357672785</v>
       </c>
       <c r="G14" t="n">
         <v>1</v>
@@ -814,13 +814,13 @@
         <v>14</v>
       </c>
       <c r="D15" t="n">
-        <v>109.461084942359</v>
+        <v>204.413127015303</v>
       </c>
       <c r="E15" t="n">
-        <v>18.7921718052805</v>
+        <v>106.907756757276</v>
       </c>
       <c r="F15" t="n">
-        <v>311.342216166098</v>
+        <v>434.060730444603</v>
       </c>
       <c r="G15" t="n">
         <v>1</v>
@@ -843,13 +843,13 @@
         <v>15</v>
       </c>
       <c r="D16" t="n">
-        <v>96.0282427799108</v>
+        <v>147.522904825849</v>
       </c>
       <c r="E16" t="n">
-        <v>31.3882622666565</v>
+        <v>85.0514608735944</v>
       </c>
       <c r="F16" t="n">
-        <v>231.306803192836</v>
+        <v>233.826154721825</v>
       </c>
       <c r="G16" t="n">
         <v>1</v>
@@ -872,16 +872,16 @@
         <v>11</v>
       </c>
       <c r="D17" t="n">
-        <v>2.88202479547351</v>
+        <v>3.98639749452161</v>
       </c>
       <c r="E17" t="n">
-        <v>-1.06378557415534</v>
+        <v>0.69864422689744</v>
       </c>
       <c r="F17" t="n">
-        <v>6.82851550609846</v>
+        <v>7.54413189225096</v>
       </c>
       <c r="G17" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H17" t="n">
         <v>9147.52631578947</v>
@@ -901,13 +901,13 @@
         <v>12</v>
       </c>
       <c r="D18" t="n">
-        <v>14.4617030721867</v>
+        <v>21.785328233901</v>
       </c>
       <c r="E18" t="n">
-        <v>0.80682614877468</v>
+        <v>13.516708171832</v>
       </c>
       <c r="F18" t="n">
-        <v>33.2700634848472</v>
+        <v>31.8467795250282</v>
       </c>
       <c r="G18" t="n">
         <v>1</v>
@@ -930,13 +930,13 @@
         <v>13</v>
       </c>
       <c r="D19" t="n">
-        <v>53.8895366420605</v>
+        <v>76.0688266715239</v>
       </c>
       <c r="E19" t="n">
-        <v>22.8956730987238</v>
+        <v>52.254380206788</v>
       </c>
       <c r="F19" t="n">
-        <v>102.252081281219</v>
+        <v>104.80959814208</v>
       </c>
       <c r="G19" t="n">
         <v>1</v>
@@ -959,16 +959,16 @@
         <v>14</v>
       </c>
       <c r="D20" t="n">
-        <v>31.1455490079015</v>
+        <v>67.285325009361</v>
       </c>
       <c r="E20" t="n">
-        <v>-4.9335024244625</v>
+        <v>30.5152582497989</v>
       </c>
       <c r="F20" t="n">
-        <v>100.829414994833</v>
+        <v>116.452643513778</v>
       </c>
       <c r="G20" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H20" t="n">
         <v>284.105263157895</v>
@@ -988,13 +988,13 @@
         <v>15</v>
       </c>
       <c r="D21" t="n">
-        <v>-39.6288120312716</v>
+        <v>-43.3778103466629</v>
       </c>
       <c r="E21" t="n">
-        <v>-48.263826304601</v>
+        <v>-48.7866056217417</v>
       </c>
       <c r="F21" t="n">
-        <v>-27.7205680786646</v>
+        <v>-37.3549402776375</v>
       </c>
       <c r="G21" t="n">
         <v>1</v>

</xml_diff>

<commit_message>
Updated commit - this might be correct for intervention date (lines appear to match but needs checking)
</commit_message>
<xml_diff>
--- a/Outputs/WY/Results.xlsx
+++ b/Outputs/WY/Results.xlsx
@@ -437,13 +437,13 @@
         <v>11</v>
       </c>
       <c r="D2" t="n">
-        <v>4.55194436134888</v>
+        <v>4.44639156119888</v>
       </c>
       <c r="E2" t="n">
-        <v>0.0563609197510995</v>
+        <v>0.0761924489145183</v>
       </c>
       <c r="F2" t="n">
-        <v>9.45954957352126</v>
+        <v>8.96780899395303</v>
       </c>
       <c r="G2" t="n">
         <v>1</v>
@@ -466,13 +466,13 @@
         <v>12</v>
       </c>
       <c r="D3" t="n">
-        <v>-1.648950251367</v>
+        <v>-1.86516394141668</v>
       </c>
       <c r="E3" t="n">
-        <v>-13.5052864425289</v>
+        <v>-13.2224611827265</v>
       </c>
       <c r="F3" t="n">
-        <v>11.2187000547253</v>
+        <v>12.1858145640159</v>
       </c>
       <c r="G3" t="n">
         <v>0</v>
@@ -495,13 +495,13 @@
         <v>13</v>
       </c>
       <c r="D4" t="n">
-        <v>-6.97982475932386</v>
+        <v>-6.68901794185942</v>
       </c>
       <c r="E4" t="n">
-        <v>-16.6459358443617</v>
+        <v>-15.7954745928014</v>
       </c>
       <c r="F4" t="n">
-        <v>4.74889646073614</v>
+        <v>4.27847252222769</v>
       </c>
       <c r="G4" t="n">
         <v>0</v>
@@ -524,13 +524,13 @@
         <v>14</v>
       </c>
       <c r="D5" t="n">
-        <v>-1.44699984262765</v>
+        <v>-1.41548574072862</v>
       </c>
       <c r="E5" t="n">
-        <v>-19.6318810745464</v>
+        <v>-18.50287152233</v>
       </c>
       <c r="F5" t="n">
-        <v>21.0400122736455</v>
+        <v>21.6222072025779</v>
       </c>
       <c r="G5" t="n">
         <v>0</v>
@@ -553,13 +553,13 @@
         <v>15</v>
       </c>
       <c r="D6" t="n">
-        <v>-45.9166131821395</v>
+        <v>-46.0478700391514</v>
       </c>
       <c r="E6" t="n">
-        <v>-52.1196125977235</v>
+        <v>-52.3867737756833</v>
       </c>
       <c r="F6" t="n">
-        <v>-38.2501219701516</v>
+        <v>-38.2439332124747</v>
       </c>
       <c r="G6" t="n">
         <v>1</v>
@@ -582,13 +582,13 @@
         <v>11</v>
       </c>
       <c r="D7" t="n">
-        <v>20.3167387785498</v>
+        <v>20.3184764543881</v>
       </c>
       <c r="E7" t="n">
-        <v>13.2842041030328</v>
+        <v>13.3678609917057</v>
       </c>
       <c r="F7" t="n">
-        <v>28.686158084496</v>
+        <v>28.0738401819582</v>
       </c>
       <c r="G7" t="n">
         <v>1</v>
@@ -611,13 +611,13 @@
         <v>12</v>
       </c>
       <c r="D8" t="n">
-        <v>21.3210454396107</v>
+        <v>21.3665435504278</v>
       </c>
       <c r="E8" t="n">
-        <v>12.0020624217291</v>
+        <v>11.7030444434211</v>
       </c>
       <c r="F8" t="n">
-        <v>31.4976304702006</v>
+        <v>32.4320452360681</v>
       </c>
       <c r="G8" t="n">
         <v>1</v>
@@ -640,13 +640,13 @@
         <v>13</v>
       </c>
       <c r="D9" t="n">
-        <v>57.6830514671484</v>
+        <v>58.3085560463384</v>
       </c>
       <c r="E9" t="n">
-        <v>31.8625096642734</v>
+        <v>31.879499682191</v>
       </c>
       <c r="F9" t="n">
-        <v>91.9316233452192</v>
+        <v>92.7027863266992</v>
       </c>
       <c r="G9" t="n">
         <v>1</v>
@@ -669,13 +669,13 @@
         <v>14</v>
       </c>
       <c r="D10" t="n">
-        <v>56.8380396682825</v>
+        <v>56.0790369227965</v>
       </c>
       <c r="E10" t="n">
-        <v>29.6456058789541</v>
+        <v>29.1024353677409</v>
       </c>
       <c r="F10" t="n">
-        <v>90.2060849455851</v>
+        <v>89.4324283429678</v>
       </c>
       <c r="G10" t="n">
         <v>1</v>
@@ -698,13 +698,13 @@
         <v>15</v>
       </c>
       <c r="D11" t="n">
-        <v>-16.5365931509972</v>
+        <v>-16.7507244450744</v>
       </c>
       <c r="E11" t="n">
-        <v>-25.1675826809712</v>
+        <v>-25.5953670402394</v>
       </c>
       <c r="F11" t="n">
-        <v>-5.90321396800044</v>
+        <v>-6.91032298469087</v>
       </c>
       <c r="G11" t="n">
         <v>1</v>
@@ -727,13 +727,13 @@
         <v>11</v>
       </c>
       <c r="D12" t="n">
-        <v>3.39013510432004</v>
+        <v>3.46560385189091</v>
       </c>
       <c r="E12" t="n">
-        <v>-0.692014453713557</v>
+        <v>-0.788958373958267</v>
       </c>
       <c r="F12" t="n">
-        <v>7.89734044144451</v>
+        <v>7.99332981257991</v>
       </c>
       <c r="G12" t="n">
         <v>0</v>
@@ -756,13 +756,13 @@
         <v>12</v>
       </c>
       <c r="D13" t="n">
-        <v>19.8336351311463</v>
+        <v>19.8519255937185</v>
       </c>
       <c r="E13" t="n">
-        <v>7.29071820799665</v>
+        <v>6.96088992711155</v>
       </c>
       <c r="F13" t="n">
-        <v>33.9609753181257</v>
+        <v>34.8723485490505</v>
       </c>
       <c r="G13" t="n">
         <v>1</v>
@@ -785,13 +785,13 @@
         <v>13</v>
       </c>
       <c r="D14" t="n">
-        <v>122.247679917388</v>
+        <v>121.366351155699</v>
       </c>
       <c r="E14" t="n">
-        <v>65.5287541530487</v>
+        <v>62.3007149282717</v>
       </c>
       <c r="F14" t="n">
-        <v>223.377357672785</v>
+        <v>218.09263915608</v>
       </c>
       <c r="G14" t="n">
         <v>1</v>
@@ -814,13 +814,13 @@
         <v>14</v>
       </c>
       <c r="D15" t="n">
-        <v>204.413127015303</v>
+        <v>200.722797698643</v>
       </c>
       <c r="E15" t="n">
-        <v>106.907756757276</v>
+        <v>104.674543316441</v>
       </c>
       <c r="F15" t="n">
-        <v>434.060730444603</v>
+        <v>412.555646794438</v>
       </c>
       <c r="G15" t="n">
         <v>1</v>
@@ -843,13 +843,13 @@
         <v>15</v>
       </c>
       <c r="D16" t="n">
-        <v>147.522904825849</v>
+        <v>147.573628946911</v>
       </c>
       <c r="E16" t="n">
-        <v>85.0514608735944</v>
+        <v>87.0798799347481</v>
       </c>
       <c r="F16" t="n">
-        <v>233.826154721825</v>
+        <v>233.069670404704</v>
       </c>
       <c r="G16" t="n">
         <v>1</v>
@@ -872,13 +872,13 @@
         <v>11</v>
       </c>
       <c r="D17" t="n">
-        <v>3.98639749452161</v>
+        <v>4.02986896349452</v>
       </c>
       <c r="E17" t="n">
-        <v>0.69864422689744</v>
+        <v>0.911993207208108</v>
       </c>
       <c r="F17" t="n">
-        <v>7.54413189225096</v>
+        <v>7.57834103758783</v>
       </c>
       <c r="G17" t="n">
         <v>1</v>
@@ -901,13 +901,13 @@
         <v>12</v>
       </c>
       <c r="D18" t="n">
-        <v>21.785328233901</v>
+        <v>21.963526903103</v>
       </c>
       <c r="E18" t="n">
-        <v>13.516708171832</v>
+        <v>12.8331585417013</v>
       </c>
       <c r="F18" t="n">
-        <v>31.8467795250282</v>
+        <v>31.3956220592159</v>
       </c>
       <c r="G18" t="n">
         <v>1</v>
@@ -930,13 +930,13 @@
         <v>13</v>
       </c>
       <c r="D19" t="n">
-        <v>76.0688266715239</v>
+        <v>76.12957440222</v>
       </c>
       <c r="E19" t="n">
-        <v>52.254380206788</v>
+        <v>53.5823162808539</v>
       </c>
       <c r="F19" t="n">
-        <v>104.80959814208</v>
+        <v>105.083739896449</v>
       </c>
       <c r="G19" t="n">
         <v>1</v>
@@ -959,13 +959,13 @@
         <v>14</v>
       </c>
       <c r="D20" t="n">
-        <v>67.285325009361</v>
+        <v>67.0693481217225</v>
       </c>
       <c r="E20" t="n">
-        <v>30.5152582497989</v>
+        <v>31.6880029015119</v>
       </c>
       <c r="F20" t="n">
-        <v>116.452643513778</v>
+        <v>119.144091419085</v>
       </c>
       <c r="G20" t="n">
         <v>1</v>
@@ -988,13 +988,13 @@
         <v>15</v>
       </c>
       <c r="D21" t="n">
-        <v>-43.3778103466629</v>
+        <v>-43.5184735099785</v>
       </c>
       <c r="E21" t="n">
-        <v>-48.7866056217417</v>
+        <v>-49.0181133405591</v>
       </c>
       <c r="F21" t="n">
-        <v>-37.3549402776375</v>
+        <v>-36.8618504623877</v>
       </c>
       <c r="G21" t="n">
         <v>1</v>

</xml_diff>